<commit_message>
Changing some Processor properties to fit in a single dictionary. Changing location to Geolocation for musiasem concepts to have ref and code. Other little changes and fixes.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/test_spreadsheet_4.xlsx
+++ b/backend_tests/z_input_files/test_spreadsheet_4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">V0.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Name</t>
+    <t xml:space="preserve">Parameter</t>
   </si>
   <si>
     <t xml:space="preserve">Value</t>
@@ -506,13 +506,13 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
@@ -641,8 +641,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -654,8 +654,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -713,8 +713,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -732,7 +732,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.2"/>
@@ -1881,8 +1881,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1903,7 +1903,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.67"/>
@@ -2153,8 +2153,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2174,11 +2174,11 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
@@ -2375,8 +2375,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>